<commit_message>
excel file to track runs
</commit_message>
<xml_diff>
--- a/best_parameters_IP.xlsx
+++ b/best_parameters_IP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>best_brick</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>lot_size</t>
+  </si>
+  <si>
+    <t>lot size options</t>
   </si>
   <si>
     <t>1-21</t>
@@ -470,7 +473,9 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" s="4">
         <v>2024</v>
       </c>
@@ -501,7 +506,7 @@
         <v>20</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H2" s="8">
         <v>2930645.56</v>
@@ -533,7 +538,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H3" s="4">
         <v>403040</v>
@@ -565,7 +570,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4" s="8">
         <v>451259.99</v>

</xml_diff>

<commit_message>
added the last run to the list with a higher minimum brick_size of 0.00005
</commit_message>
<xml_diff>
--- a/best_parameters_IP.xlsx
+++ b/best_parameters_IP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>best_brick</t>
   </si>
@@ -61,13 +61,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -110,20 +110,20 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -436,7 +436,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -449,12 +449,12 @@
     <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="10" width="8.43357142857143" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="18.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,57 +487,57 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="5">
+      <c r="A2" s="1">
         <v>0.00001</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="1">
         <v>0.1156</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="1">
         <v>0.3089</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="2">
         <v>65</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="2">
         <v>5</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="2">
         <v>20</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="6">
         <v>2930645.56</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="6">
         <v>33552970.14</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="6">
         <v>53863825.47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="5">
+      <c r="A3" s="1">
         <v>0.00001</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="1">
         <v>0.1907</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="1">
         <v>0.323999999999999</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="2">
         <v>10</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="1">
         <v>7.5</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="2">
         <v>4</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="4">
@@ -550,36 +550,68 @@
         <v>9124250</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1">
         <v>0.00003</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="1">
         <v>0.1788</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="1">
         <v>0.276999999999999</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="2">
         <v>12</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="1">
         <v>3.5</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="2">
         <v>5</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="6">
         <v>451259.99</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="6">
         <v>5443904.99</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="6">
         <v>9662459.99</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="7">
+        <v>0.00007</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.1502</v>
+      </c>
+      <c r="C5" s="7">
+        <v>273</v>
+      </c>
+      <c r="D5" s="8">
+        <v>12.66</v>
+      </c>
+      <c r="E5" s="7">
+        <v>3.166</v>
+      </c>
+      <c r="F5" s="8">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="7">
+        <v>214665</v>
+      </c>
+      <c r="I5" s="7">
+        <v>2628385</v>
+      </c>
+      <c r="J5" s="7">
+        <v>5008870</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added most recent run
</commit_message>
<xml_diff>
--- a/best_parameters_IP.xlsx
+++ b/best_parameters_IP.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>best_brick</t>
   </si>
@@ -37,6 +37,27 @@
     <t>lot size options</t>
   </si>
   <si>
+    <t>best_inc</t>
+  </si>
+  <si>
+    <t>best_max</t>
+  </si>
+  <si>
+    <t>best_ma</t>
+  </si>
+  <si>
+    <t>best_signal</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
     <t>1-21</t>
   </si>
   <si>
@@ -44,6 +65,15 @@
   </si>
   <si>
     <t>set to 5</t>
+  </si>
+  <si>
+    <t>(3566419.9999995492, 0)</t>
+  </si>
+  <si>
+    <t>(1831444.99999976, 2)</t>
+  </si>
+  <si>
+    <t>(150629.99999998, 0)</t>
   </si>
 </sst>
 </file>
@@ -60,6 +90,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -80,12 +111,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -99,39 +145,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
@@ -159,28 +214,28 @@
         <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -436,25 +491,32 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="8.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +526,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -476,174 +538,269 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="2">
         <v>2024</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="2">
         <v>2023</v>
       </c>
-      <c r="J1" s="4">
+      <c r="J1" s="2">
         <v>2022</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="4">
         <v>0.00001</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>0.1156</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>0.3089</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="5">
         <v>65</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="5">
         <v>5</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="5">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="6">
+      <c r="G2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4">
         <v>2930645.56</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="4">
         <v>33552970.14</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="4">
         <v>53863825.47</v>
       </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="4">
         <v>0.00001</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>0.1907</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>0.323999999999999</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="5">
         <v>10</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <v>7.5</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="5">
         <v>4</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="G3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="5">
         <v>403040</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="5">
         <v>4934702</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="5">
         <v>9124250</v>
       </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1">
+      <c r="A4" s="4">
         <v>0.00003</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>0.1788</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>0.276999999999999</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="5">
         <v>12</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>3.5</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="5">
         <v>5</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="G4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="4">
         <v>451259.99</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="4">
         <v>5443904.99</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="4">
         <v>9662459.99</v>
       </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="7">
+      <c r="A5" s="4">
         <v>0.00007</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="4">
         <v>0.1502</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>273</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="4">
         <v>12.66</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="4">
         <v>3.166</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="5">
         <v>5</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="7">
+      <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="5">
         <v>214665</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5">
         <v>2628385</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="5">
         <v>5008870</v>
       </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="7">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="4">
         <v>0.000079</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="4">
         <v>0.1467</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>0.3669</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="4">
         <v>12.85</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="4">
         <v>3.86</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="5">
         <v>5</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="7">
+      <c r="G6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="5">
         <v>187190</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="5">
         <v>2287365</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="5">
         <v>4206735</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="4">
+        <v>0.0001</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="5">
+        <v>5</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="4">
+        <v>0.1729000000000001</v>
+      </c>
+      <c r="L7" s="4">
+        <v>0.231886569187853</v>
+      </c>
+      <c r="M7" s="4">
+        <v>9.954991948907438</v>
+      </c>
+      <c r="N7" s="4">
+        <v>3.996463222662106</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the latest run and fixed the column naming error
</commit_message>
<xml_diff>
--- a/best_parameters_IP.xlsx
+++ b/best_parameters_IP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WilliamFetzner\Documents\Trading\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE957C5A-400C-4476-8D1F-2148821F2D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03471247-E81C-4EAA-BBC6-11AE6C8F23C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17325" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,27 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>best_brick</t>
   </si>
   <si>
+    <t>best_inc</t>
+  </si>
+  <si>
+    <t>best_max</t>
+  </si>
+  <si>
+    <t>best_ma</t>
+  </si>
+  <si>
+    <t>best_signal</t>
+  </si>
+  <si>
     <t>lot_size</t>
   </si>
   <si>
     <t>lot size options</t>
   </si>
   <si>
-    <t>best_inc</t>
-  </si>
-  <si>
-    <t>best_max</t>
-  </si>
-  <si>
-    <t>best_ma</t>
-  </si>
-  <si>
-    <t>best_signal</t>
+    <t>3 months</t>
   </si>
   <si>
     <t>1-21</t>
@@ -417,35 +420,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="H1" s="1">
         <v>2024</v>
@@ -456,8 +459,11 @@
       <c r="J1" s="1">
         <v>2022</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.0000000000000001E-5</v>
       </c>
@@ -477,7 +483,7 @@
         <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <v>2930645.56</v>
@@ -489,7 +495,7 @@
         <v>53863825.469999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.0000000000000001E-5</v>
       </c>
@@ -509,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H3">
         <v>403040</v>
@@ -521,7 +527,7 @@
         <v>9124250</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3.0000000000000001E-5</v>
       </c>
@@ -541,7 +547,7 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H4">
         <v>451259.99</v>
@@ -553,7 +559,7 @@
         <v>9662459.9900000002</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6.9999999999999994E-5</v>
       </c>
@@ -573,7 +579,7 @@
         <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H5">
         <v>214665</v>
@@ -585,7 +591,7 @@
         <v>5008870</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7.8999999999999996E-5</v>
       </c>
@@ -605,7 +611,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H6">
         <v>187190</v>
@@ -617,7 +623,7 @@
         <v>4206735</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1E-4</v>
       </c>
@@ -637,7 +643,7 @@
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H7">
         <v>150629.99</v>
@@ -649,7 +655,7 @@
         <v>3566419.99</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1E-4</v>
       </c>
@@ -669,7 +675,7 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H8">
         <v>150419.99</v>
@@ -679,6 +685,41 @@
       </c>
       <c r="J8">
         <v>3535944.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="B9">
+        <v>8.8951110248452342E-4</v>
+      </c>
+      <c r="C9">
+        <v>0.2129999999999998</v>
+      </c>
+      <c r="D9">
+        <v>64</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>